<commit_message>
Baseline to third order, partial GP implementation
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE3F110-C084-4EC9-8BF0-2E1501138B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B68A89-00F7-45F6-B4CB-06244BD8C3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="92">
   <si>
     <t>Category</t>
   </si>
@@ -248,6 +248,60 @@
   </si>
   <si>
     <t>(4)+correction factor</t>
+  </si>
+  <si>
+    <t>f9fb</t>
+  </si>
+  <si>
+    <t>(4)+ecc tweaked</t>
+  </si>
+  <si>
+    <t>No correction factor is needed</t>
+  </si>
+  <si>
+    <t>Huh? Still conclude we need it</t>
+  </si>
+  <si>
+    <t>No eccentricity</t>
+  </si>
+  <si>
+    <t>(4)+don't mask hot</t>
+  </si>
+  <si>
+    <t>(4)+don't remove background rows</t>
+  </si>
+  <si>
+    <t>(4)+no flat field correction</t>
+  </si>
+  <si>
+    <t>Doesn't matter on train, bad on test</t>
+  </si>
+  <si>
+    <t>(4)+sigma clip 10</t>
+  </si>
+  <si>
+    <t>(4)+sigma clip 4</t>
+  </si>
+  <si>
+    <t>(4)+sigma clip 6</t>
+  </si>
+  <si>
+    <t>(5)+12 background rows</t>
+  </si>
+  <si>
+    <t>Makes no sense...</t>
+  </si>
+  <si>
+    <t>12,13,14</t>
+  </si>
+  <si>
+    <t>12,13,14 - weird…</t>
+  </si>
+  <si>
+    <t>(5)+4 background rows</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
@@ -314,7 +368,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CA98BC4-9283-42D5-A195-DA0C9C245AC9}" name="Table1" displayName="Table1" ref="A1:F22" totalsRowShown="0">
-  <autoFilter ref="A1:F22" xr:uid="{6CA98BC4-9283-42D5-A195-DA0C9C245AC9}"/>
+  <autoFilter ref="A1:F22" xr:uid="{6CA98BC4-9283-42D5-A195-DA0C9C245AC9}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Verify"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B6616B63-F1E7-417B-975B-CF7294D71629}" name="Category"/>
     <tableColumn id="2" xr3:uid="{8F4FDD69-72A5-4F1F-ABA4-5AAD37F6314F}" name="Choice"/>
@@ -328,8 +388,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:M9" totalsRowShown="0">
-  <autoFilter ref="A1:M9" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:M19" totalsRowShown="0">
+  <autoFilter ref="A1:M19" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -649,7 +709,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -700,7 +760,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
@@ -709,8 +769,14 @@
       <c r="D3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -724,7 +790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -741,7 +807,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -752,7 +818,13 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>68</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -766,21 +838,33 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -811,21 +895,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -867,35 +957,47 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>6.5</v>
+      </c>
+      <c r="F15">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -915,7 +1017,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -929,7 +1031,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -943,7 +1045,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -957,7 +1059,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -971,7 +1073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -995,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1108,7 @@
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1175,7 +1277,7 @@
       <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>0.42209999999999998</v>
       </c>
       <c r="J5" s="2">
@@ -1184,7 +1286,7 @@
       <c r="K5" s="2">
         <v>495.4</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>0.39100000000000001</v>
       </c>
       <c r="M5" t="s">
@@ -1248,33 +1350,39 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
         <v>27</v>
       </c>
       <c r="I8">
-        <v>0.41880000000000001</v>
+        <v>0.41060000000000002</v>
       </c>
       <c r="J8">
-        <v>260.39999999999998</v>
+        <v>275.8</v>
       </c>
       <c r="K8">
-        <v>499.1</v>
+        <v>521.6</v>
+      </c>
+      <c r="L8">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="M8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -1283,10 +1391,321 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9">
+        <v>0.4204</v>
+      </c>
+      <c r="J9">
+        <v>255.6</v>
+      </c>
+      <c r="K9">
+        <v>497</v>
+      </c>
+      <c r="L9">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="M9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10">
+        <v>0.41880000000000001</v>
+      </c>
+      <c r="J10">
+        <v>260.39999999999998</v>
+      </c>
+      <c r="K10">
+        <v>499.1</v>
+      </c>
+      <c r="L10">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="M10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <v>0.42349999999999999</v>
+      </c>
+      <c r="J11">
+        <v>219.8</v>
+      </c>
+      <c r="K11">
+        <v>495.7</v>
+      </c>
+      <c r="L11">
+        <v>0.37</v>
+      </c>
+      <c r="M11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12">
+        <v>0.4219</v>
+      </c>
+      <c r="J12">
+        <v>235.6</v>
+      </c>
+      <c r="K12">
+        <v>496.9</v>
+      </c>
+      <c r="L12">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="M12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13">
+        <v>0.42009999999999997</v>
+      </c>
+      <c r="J13">
+        <v>261.89999999999998</v>
+      </c>
+      <c r="K13">
+        <v>495.8</v>
+      </c>
+      <c r="L13">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="M13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14">
+        <v>0.4214</v>
+      </c>
+      <c r="J14">
+        <v>243.6</v>
+      </c>
+      <c r="K14">
+        <v>496.6</v>
+      </c>
+      <c r="L14">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15">
+        <v>0.42309999999999998</v>
+      </c>
+      <c r="J15">
+        <v>222.2</v>
+      </c>
+      <c r="K15">
+        <v>496.5</v>
+      </c>
+      <c r="L15">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16">
+        <v>0.4229</v>
+      </c>
+      <c r="J16">
+        <v>229.4</v>
+      </c>
+      <c r="K16">
+        <v>495.4</v>
+      </c>
+      <c r="L16">
+        <v>0.36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17">
+        <v>0.4194</v>
+      </c>
+      <c r="J17">
+        <v>226.8</v>
+      </c>
+      <c r="K17">
+        <v>506.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="J18">
+        <v>231.8</v>
+      </c>
+      <c r="K18">
+        <v>496.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <v>0.42159999999999997</v>
+      </c>
+      <c r="G19">
+        <v>237.4</v>
+      </c>
+      <c r="H19">
+        <v>496.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sanity checks to parallel runs
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAC3FC3-71D7-4078-BE5F-B5D5DBF61442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2687CCD2-8679-4D59-ACC0-3A61C386D419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="117">
   <si>
     <t>Category</t>
   </si>
@@ -375,9 +375,6 @@
   </si>
   <si>
     <t>Linux lim=1</t>
-  </si>
-  <si>
-    <t>Sanity check</t>
   </si>
   <si>
     <t>Two above cvombined</t>
@@ -1903,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBBA9B5-89A0-4EDA-AA5C-6A06A9856157}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,12 +1912,12 @@
     <col min="9" max="10" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>102</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -1977,8 +1974,12 @@
         <f>K4/4</f>
         <v>0.35416666666666669</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <f>60*K4</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>1.5333333333333332</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>0.43333333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -2067,8 +2068,8 @@
       <c r="D8">
         <v>368.6</v>
       </c>
-      <c r="E8" t="s">
-        <v>116</v>
+      <c r="E8">
+        <v>0.23200000000000001</v>
       </c>
       <c r="H8">
         <v>7</v>
@@ -2081,17 +2082,39 @@
         <v>1.6166666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9">
         <f>B7+B8-B6</f>
         <v>0.51749999999999996</v>
       </c>
-      <c r="E9" t="e">
+      <c r="E9">
         <f>E7+E8-E6</f>
-        <v>#VALUE!</v>
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="S9">
+        <f>87/126*3/2</f>
+        <v>1.0357142857142856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <f>73/87*4/3</f>
+        <v>1.1187739463601531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <f>3/4</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S14">
+        <f>73/87</f>
+        <v>0.83908045977011492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add limb darkening parameter slope to AIRS
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2687CCD2-8679-4D59-ACC0-3A61C386D419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082D9E46-9C03-49AE-8DB2-8C7E224A30C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -1187,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1846,7 @@
         <v>495.5</v>
       </c>
       <c r="L20">
-        <v>3.379</v>
+        <v>0.379</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBBA9B5-89A0-4EDA-AA5C-6A06A9856157}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Stop fixing AIRS sigma for GP
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082D9E46-9C03-49AE-8DB2-8C7E224A30C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855CD2E-3F28-49CB-BB34-4879C8E83F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
   <si>
     <t>Category</t>
   </si>
@@ -378,6 +378,24 @@
   </si>
   <si>
     <t>Two above cvombined</t>
+  </si>
+  <si>
+    <t>7262</t>
+  </si>
+  <si>
+    <t>(19)+No bad planet in train</t>
+  </si>
+  <si>
+    <t>(20)+No background removal</t>
+  </si>
+  <si>
+    <t>(21)+Time binning before full sensor</t>
+  </si>
+  <si>
+    <t>a24c</t>
+  </si>
+  <si>
+    <t>ce9e</t>
   </si>
 </sst>
 </file>
@@ -476,8 +494,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:M21" totalsRowShown="0">
-  <autoFilter ref="A1:M21" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:M24" totalsRowShown="0">
+  <autoFilter ref="A1:M24" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -1185,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,7 +1799,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
@@ -1888,6 +1906,84 @@
       </c>
       <c r="M21" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>0.42230000000000001</v>
+      </c>
+      <c r="G22">
+        <v>236.3</v>
+      </c>
+      <c r="H22">
+        <v>495.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23">
+        <v>0.42259999999999998</v>
+      </c>
+      <c r="G23">
+        <v>221</v>
+      </c>
+      <c r="H23">
+        <v>498.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <v>0.42259999999999998</v>
+      </c>
+      <c r="G24">
+        <v>221.1</v>
+      </c>
+      <c r="H24">
+        <v>498.4</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +1999,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New mean correction available, not default
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D643EE0A-C6B4-4BD8-9BE0-4C2325B5B9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806A9E3F-7D94-4630-8EEA-BCD600572EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="149">
   <si>
     <t>Category</t>
   </si>
@@ -463,6 +463,18 @@
   </si>
   <si>
     <t>CV20</t>
+  </si>
+  <si>
+    <t>CV20K</t>
+  </si>
+  <si>
+    <t>RUNNING</t>
+  </si>
+  <si>
+    <t>7838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -561,9 +573,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:N26" totalsRowShown="0">
-  <autoFilter ref="A1:N26" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O27" totalsRowShown="0">
+  <autoFilter ref="A1:O27" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
     <tableColumn id="12" xr3:uid="{F6596AEB-9D64-4014-88C3-3FBD71A31D55}" name="Over"/>
@@ -573,6 +585,7 @@
     <tableColumn id="5" xr3:uid="{ADA1A98F-3920-41D3-BAA1-B8AE26FFD47F}" name="CV loc"/>
     <tableColumn id="8" xr3:uid="{6CF4D6D5-8CEB-444F-A2A2-3A2A90BFAC66}" name="RMSF loc"/>
     <tableColumn id="10" xr3:uid="{36A8478E-9821-4ACA-9D75-7D077500894E}" name="RMSA loc"/>
+    <tableColumn id="15" xr3:uid="{4872B848-2CDF-4034-A7D8-381009C570B8}" name="CV20K"/>
     <tableColumn id="6" xr3:uid="{6CF5D5A7-DD58-4784-AE79-32A028248CBE}" name="CV kag"/>
     <tableColumn id="9" xr3:uid="{C287B71C-494C-4903-93AA-2F5669CE90AC}" name="RMSF kag"/>
     <tableColumn id="11" xr3:uid="{060A4CB9-C965-40F8-B5CF-1088C09879A9}" name="RMSA kag"/>
@@ -1271,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,15 +1301,16 @@
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.85546875" customWidth="1"/>
-    <col min="15" max="15" width="6" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1325,22 +1339,25 @@
         <v>49</v>
       </c>
       <c r="J1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1359,17 +1376,17 @@
       <c r="G2">
         <v>0.41249999999999998</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.41270000000000001</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.39400000000000002</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1395,23 +1412,23 @@
       <c r="I3">
         <v>498.7</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.41770000000000002</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>297.3</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>497.7</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.39200000000000002</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1428,20 +1445,20 @@
         <v>25</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="J4">
+      <c r="K4">
         <v>0.42020000000000002</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>265.10000000000002</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>496.3</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1458,23 +1475,23 @@
         <v>27</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="J5">
+      <c r="K5">
         <v>0.42209999999999998</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>238.5</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>495.4</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.39100000000000001</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1491,20 +1508,20 @@
         <v>27</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="J6">
+      <c r="K6">
         <v>0.41170000000000001</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>273.60000000000002</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>518.4</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.38200000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1521,17 +1538,17 @@
         <v>27</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="J7">
+      <c r="K7">
         <v>0.42180000000000001</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>234.5</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>496.8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.5</v>
       </c>
@@ -1547,23 +1564,23 @@
       <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.41060000000000002</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>275.8</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>521.6</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0.38100000000000001</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1580,23 +1597,23 @@
         <v>27</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="J9">
+      <c r="K9">
         <v>0.4204</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>255.6</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>497</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0.39200000000000002</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1613,23 +1630,23 @@
         <v>27</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="J10">
+      <c r="K10">
         <v>0.41880000000000001</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>260.39999999999998</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>499.1</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.38900000000000001</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1646,23 +1663,23 @@
         <v>27</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="J11">
+      <c r="K11">
         <v>0.42349999999999999</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>219.8</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>495.7</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0.37</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1679,23 +1696,23 @@
         <v>27</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="J12">
+      <c r="K12">
         <v>0.4219</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>235.6</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>496.9</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>0.35099999999999998</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1712,23 +1729,23 @@
         <v>27</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="J13">
+      <c r="K13">
         <v>0.42009999999999997</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>261.89999999999998</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>495.8</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>0.36399999999999999</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1745,20 +1762,20 @@
         <v>27</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="J14">
+      <c r="K14">
         <v>0.4214</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>243.6</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>496.6</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1775,20 +1792,20 @@
         <v>27</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="J15">
+      <c r="K15">
         <v>0.42309999999999998</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>222.2</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>496.5</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>0.37</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1805,23 +1822,23 @@
         <v>27</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="J16">
+      <c r="K16">
         <v>0.4229</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>229.4</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>495.4</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>0.36</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1838,17 +1855,17 @@
         <v>27</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="J17">
+      <c r="K17">
         <v>0.4194</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>226.8</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>506.3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1865,17 +1882,17 @@
         <v>27</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="J18">
+      <c r="K18">
         <v>0.42209999999999998</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>231.8</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>496.8</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1900,23 +1917,23 @@
       <c r="I19">
         <v>496.7</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>0.42209999999999998</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>238.5</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>495.4</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>0.39100000000000001</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1941,20 +1958,20 @@
       <c r="I20">
         <v>494.9</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.42349999999999999</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>220.6</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>495.5</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>0.379</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1979,23 +1996,24 @@
       <c r="I21" s="2">
         <v>495.2</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2">
         <v>0.42049999999999998</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>229.5</v>
       </c>
-      <c r="L21" s="2">
+      <c r="M21" s="2">
         <v>501.8</v>
       </c>
-      <c r="M21" s="2">
+      <c r="N21" s="2">
         <v>0.372</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2021,7 +2039,7 @@
         <v>495.4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2047,7 +2065,7 @@
         <v>498.4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2072,23 +2090,23 @@
       <c r="I24">
         <v>498.4</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>0.42259999999999998</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>223.1</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>497.9</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>0.35699999999999998</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2116,19 +2134,19 @@
       <c r="I25">
         <v>163.19999999999999</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>0.59</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>141</v>
+      <c r="B26" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
         <v>143</v>
@@ -2147,6 +2165,17 @@
       </c>
       <c r="I26">
         <v>160.30000000000001</v>
+      </c>
+      <c r="J26">
+        <v>0.6119</v>
+      </c>
+      <c r="N26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New mean correction, new FGS invalid handling
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806A9E3F-7D94-4630-8EEA-BCD600572EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECC1646-08AF-435B-9FF3-90093A3FD228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="152">
   <si>
     <t>Category</t>
   </si>
@@ -468,13 +468,22 @@
     <t>CV20K</t>
   </si>
   <si>
-    <t>RUNNING</t>
-  </si>
-  <si>
     <t>7838</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
+    <t>(24)+new mean correction</t>
+  </si>
+  <si>
+    <t>07a1</t>
+  </si>
+  <si>
+    <t>New mean correction is in</t>
+  </si>
+  <si>
+    <t>(25)+new FGS invalid handling</t>
+  </si>
+  <si>
+    <t>(27)+no inpainting FGS</t>
   </si>
 </sst>
 </file>
@@ -573,8 +582,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O27" totalsRowShown="0">
-  <autoFilter ref="A1:O27" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O29" totalsRowShown="0">
+  <autoFilter ref="A1:O29" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -1284,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,7 +2152,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -2169,13 +2178,104 @@
       <c r="J26">
         <v>0.6119</v>
       </c>
-      <c r="N26" t="s">
-        <v>146</v>
+      <c r="N26">
+        <v>0.58899999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27" t="s">
         <v>148</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27">
+        <v>0.62170000000000003</v>
+      </c>
+      <c r="G27">
+        <v>0.60219999999999996</v>
+      </c>
+      <c r="H27">
+        <v>223.4</v>
+      </c>
+      <c r="I27">
+        <v>158.1</v>
+      </c>
+      <c r="J27">
+        <v>0.62239999999999995</v>
+      </c>
+      <c r="N27">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="O27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28">
+        <v>0.62350000000000005</v>
+      </c>
+      <c r="G28">
+        <v>0.60429999999999995</v>
+      </c>
+      <c r="H28">
+        <v>211</v>
+      </c>
+      <c r="I28">
+        <v>163.30000000000001</v>
+      </c>
+      <c r="J28">
+        <v>0.62429999999999997</v>
+      </c>
+      <c r="N28">
+        <v>0.59899999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>151</v>
+      </c>
+      <c r="G29">
+        <v>0.60529999999999995</v>
+      </c>
+      <c r="H29">
+        <v>211.9</v>
+      </c>
+      <c r="I29">
+        <v>163.1</v>
+      </c>
+      <c r="N29">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New AIRS prep (not yet default)
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF2DE1-D925-4F10-A636-101F0B2C17E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85E4CA6-5F4D-4AD1-A4E9-5F73740D6BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="160">
   <si>
     <t>Category</t>
   </si>
@@ -499,6 +499,15 @@
   </si>
   <si>
     <t>(29)+4 background rows</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>(29)+new AIRS inf</t>
+  </si>
+  <si>
+    <t>(29)+new AIRS 50</t>
   </si>
 </sst>
 </file>
@@ -597,8 +606,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O33" totalsRowShown="0">
-  <autoFilter ref="A1:O33" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O35" totalsRowShown="0">
+  <autoFilter ref="A1:O35" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -1308,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,6 +2415,40 @@
         <v>159.30000000000001</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
New FGS prep (not yet default)
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85E4CA6-5F4D-4AD1-A4E9-5F73740D6BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7121AF4A-1FAF-4FB3-BD61-CA3EAFE3C2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="164">
   <si>
     <t>Category</t>
   </si>
@@ -508,6 +508,18 @@
   </si>
   <si>
     <t>(29)+new AIRS 50</t>
+  </si>
+  <si>
+    <t>residuals in covariance matrix</t>
+  </si>
+  <si>
+    <t>fit residual mean</t>
+  </si>
+  <si>
+    <t>fit residual std</t>
+  </si>
+  <si>
+    <t>noise est relative to naïve</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1355,7 @@
     <col min="16" max="16" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1419,7 +1431,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1460,8 +1472,11 @@
       <c r="O3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1490,8 +1505,11 @@
       <c r="N4">
         <v>0.39200000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1523,8 +1541,11 @@
       <c r="O5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1553,8 +1574,11 @@
       <c r="N6">
         <v>0.38200000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1581,7 +1605,7 @@
         <v>496.8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.5</v>
       </c>
@@ -1613,7 +1637,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1679,7 +1703,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1712,7 +1736,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1745,7 +1769,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1778,7 +1802,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1808,7 +1832,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1838,7 +1862,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2389,7 +2413,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2415,7 +2439,7 @@
         <v>159.30000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2431,8 +2455,20 @@
       <c r="E34" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="H34">
+        <v>210.1</v>
+      </c>
+      <c r="I34">
+        <v>157</v>
+      </c>
+      <c r="N34">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2447,6 +2483,18 @@
       </c>
       <c r="E35" t="s">
         <v>25</v>
+      </c>
+      <c r="G35">
+        <v>0.60629999999999995</v>
+      </c>
+      <c r="H35">
+        <v>211</v>
+      </c>
+      <c r="I35">
+        <v>162.6</v>
+      </c>
+      <c r="N35">
+        <v>0.189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New baseline: new FGS and AIRS loaders, polynomial drift
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7121AF4A-1FAF-4FB3-BD61-CA3EAFE3C2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65B8330-28C8-400B-986C-F4E3F0BC4E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
+    <workbookView xWindow="-28800" yWindow="510" windowWidth="28800" windowHeight="15240" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="170">
   <si>
     <t>Category</t>
   </si>
@@ -520,12 +520,33 @@
   </si>
   <si>
     <t>noise est relative to naïve</t>
+  </si>
+  <si>
+    <t>(29)+no sanity checks</t>
+  </si>
+  <si>
+    <t>(29)+new FGS</t>
+  </si>
+  <si>
+    <t>0a3b</t>
+  </si>
+  <si>
+    <t>(35)+fixed FGS mean</t>
+  </si>
+  <si>
+    <t>(36)+poly FGS</t>
+  </si>
+  <si>
+    <t>(37)+new AIRS simpler noise_est</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -574,16 +595,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -618,8 +645,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O35" totalsRowShown="0">
-  <autoFilter ref="A1:O35" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:O40" totalsRowShown="0">
+  <autoFilter ref="A1:O40" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -634,7 +661,7 @@
     <tableColumn id="6" xr3:uid="{6CF5D5A7-DD58-4784-AE79-32A028248CBE}" name="CV kag"/>
     <tableColumn id="9" xr3:uid="{C287B71C-494C-4903-93AA-2F5669CE90AC}" name="RMSF kag"/>
     <tableColumn id="11" xr3:uid="{060A4CB9-C965-40F8-B5CF-1088C09879A9}" name="RMSA kag"/>
-    <tableColumn id="13" xr3:uid="{DEE7C2ED-70DD-4233-BFCD-10F248630020}" name="LB"/>
+    <tableColumn id="13" xr3:uid="{DEE7C2ED-70DD-4233-BFCD-10F248630020}" name="LB" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{3C7DE663-78E6-4BAF-B965-54D475799F16}" name="Conclusions"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1329,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,7 +1451,7 @@
       <c r="K2">
         <v>0.41270000000000001</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>0.39400000000000002</v>
       </c>
       <c r="O2" t="s">
@@ -1466,7 +1493,7 @@
       <c r="M3">
         <v>497.7</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>0.39200000000000002</v>
       </c>
       <c r="O3" t="s">
@@ -1502,7 +1529,7 @@
       <c r="M4">
         <v>496.3</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>0.39200000000000002</v>
       </c>
       <c r="T4" t="s">
@@ -1535,7 +1562,7 @@
       <c r="M5">
         <v>495.4</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>0.39100000000000001</v>
       </c>
       <c r="O5" t="s">
@@ -1571,7 +1598,7 @@
       <c r="M6">
         <v>518.4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>0.38200000000000001</v>
       </c>
       <c r="T6" t="s">
@@ -1604,6 +1631,7 @@
       <c r="M7">
         <v>496.8</v>
       </c>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1630,7 +1658,7 @@
       <c r="M8">
         <v>521.6</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="4">
         <v>0.38100000000000001</v>
       </c>
       <c r="O8" t="s">
@@ -1663,7 +1691,7 @@
       <c r="M9">
         <v>497</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>0.39200000000000002</v>
       </c>
       <c r="O9" t="s">
@@ -1696,7 +1724,7 @@
       <c r="M10">
         <v>499.1</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>0.38900000000000001</v>
       </c>
       <c r="O10" t="s">
@@ -1729,7 +1757,7 @@
       <c r="M11">
         <v>495.7</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="4">
         <v>0.37</v>
       </c>
       <c r="O11" t="s">
@@ -1762,7 +1790,7 @@
       <c r="M12">
         <v>496.9</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="4">
         <v>0.35099999999999998</v>
       </c>
       <c r="O12" t="s">
@@ -1795,7 +1823,7 @@
       <c r="M13">
         <v>495.8</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="4">
         <v>0.36399999999999999</v>
       </c>
       <c r="O13" t="s">
@@ -1828,7 +1856,7 @@
       <c r="M14">
         <v>496.6</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>0.33400000000000002</v>
       </c>
     </row>
@@ -1858,7 +1886,7 @@
       <c r="M15">
         <v>496.5</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="4">
         <v>0.37</v>
       </c>
     </row>
@@ -1888,7 +1916,7 @@
       <c r="M16">
         <v>495.4</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="4">
         <v>0.36</v>
       </c>
       <c r="O16" t="s">
@@ -1921,6 +1949,7 @@
       <c r="M17">
         <v>506.3</v>
       </c>
+      <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1948,6 +1977,7 @@
       <c r="M18">
         <v>496.8</v>
       </c>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1983,7 +2013,7 @@
       <c r="M19">
         <v>495.4</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="4">
         <v>0.39100000000000001</v>
       </c>
       <c r="O19" t="s">
@@ -2024,7 +2054,7 @@
       <c r="M20">
         <v>495.5</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <v>0.379</v>
       </c>
     </row>
@@ -2063,7 +2093,7 @@
       <c r="M21" s="2">
         <v>501.8</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="5">
         <v>0.372</v>
       </c>
       <c r="O21" t="s">
@@ -2095,6 +2125,7 @@
       <c r="I22">
         <v>495.4</v>
       </c>
+      <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2121,6 +2152,7 @@
       <c r="I23">
         <v>498.4</v>
       </c>
+      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2156,7 +2188,7 @@
       <c r="M24">
         <v>497.9</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>0.35699999999999998</v>
       </c>
       <c r="O24" t="s">
@@ -2191,7 +2223,7 @@
       <c r="I25">
         <v>163.19999999999999</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="4">
         <v>0.59</v>
       </c>
     </row>
@@ -2226,7 +2258,7 @@
       <c r="J26">
         <v>0.6119</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="4">
         <v>0.58899999999999997</v>
       </c>
     </row>
@@ -2261,7 +2293,7 @@
       <c r="J27">
         <v>0.62239999999999995</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="4">
         <v>0.59599999999999997</v>
       </c>
       <c r="O27" t="s">
@@ -2296,7 +2328,7 @@
       <c r="J28">
         <v>0.62429999999999997</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="4">
         <v>0.59899999999999998</v>
       </c>
     </row>
@@ -2322,7 +2354,7 @@
       <c r="I29">
         <v>163.1</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="4">
         <v>0.6</v>
       </c>
     </row>
@@ -2351,7 +2383,7 @@
       <c r="I30">
         <v>163.1</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="4">
         <v>0.6</v>
       </c>
     </row>
@@ -2380,7 +2412,7 @@
       <c r="I31">
         <v>162.69999999999999</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="4">
         <v>0.59699999999999998</v>
       </c>
     </row>
@@ -2409,7 +2441,7 @@
       <c r="I32">
         <v>157.69999999999999</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="4">
         <v>0.59799999999999998</v>
       </c>
     </row>
@@ -2438,6 +2470,7 @@
       <c r="I33">
         <v>159.30000000000001</v>
       </c>
+      <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -2464,7 +2497,7 @@
       <c r="I34">
         <v>157</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="4">
         <v>0.189</v>
       </c>
     </row>
@@ -2493,8 +2526,106 @@
       <c r="I35">
         <v>162.6</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="4">
         <v>0.189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>164</v>
+      </c>
+      <c r="N36" s="4">
+        <v>0.59899999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37">
+        <v>0.6079</v>
+      </c>
+      <c r="H37">
+        <v>199.05</v>
+      </c>
+      <c r="I37">
+        <v>151.75</v>
+      </c>
+      <c r="N37" s="4">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="H38">
+        <v>196.7</v>
+      </c>
+      <c r="I38">
+        <v>148.9</v>
+      </c>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39">
+        <v>0.60709999999999997</v>
+      </c>
+      <c r="H39">
+        <v>228.8</v>
+      </c>
+      <c r="I39">
+        <v>173.5</v>
+      </c>
+      <c r="N39" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40">
+        <v>0.60719999999999996</v>
+      </c>
+      <c r="H40">
+        <v>232.3</v>
+      </c>
+      <c r="I40">
+        <v>178.4</v>
+      </c>
+      <c r="N40" s="4">
+        <v>0.59899999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New baseline: fudger2, FGS-AIRS coupling
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7B3DD2-8049-403F-ADF7-A733B9FA25DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3932EDE0-8A44-4190-8A02-F858D559D23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,6 +2823,21 @@
       <c r="E45" t="s">
         <v>25</v>
       </c>
+      <c r="G45">
+        <v>0.60580000000000001</v>
+      </c>
+      <c r="H45">
+        <v>201</v>
+      </c>
+      <c r="I45">
+        <v>56.7</v>
+      </c>
+      <c r="J45">
+        <v>156.9</v>
+      </c>
+      <c r="K45">
+        <v>61.4</v>
+      </c>
       <c r="P45" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New baseline: new transit prior
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3932EDE0-8A44-4190-8A02-F858D559D23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1E5937-23DD-459E-BDFA-BCA46E31E813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,7 +2838,9 @@
       <c r="K45">
         <v>61.4</v>
       </c>
-      <c r="P45" s="4"/>
+      <c r="P45" s="4">
+        <v>0.60499999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ariel_simple2 batch 1: limit initial time search
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D06D93D-EAFA-40B1-8502-6DFC1BD6A63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF474E9-D858-4010-A8B4-2752ECD19D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="185">
   <si>
     <t>Category</t>
   </si>
@@ -577,6 +577,12 @@
   </si>
   <si>
     <t>(44)+fudger3</t>
+  </si>
+  <si>
+    <t>a029</t>
+  </si>
+  <si>
+    <t>(45)+tweak loader, fallbacks in simple, unlock t0</t>
   </si>
 </sst>
 </file>
@@ -684,8 +690,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:Q47" totalsRowShown="0">
-  <autoFilter ref="A1:Q47" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:Q48" totalsRowShown="0">
+  <autoFilter ref="A1:Q48" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -1397,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2917,7 +2923,24 @@
       <c r="K47">
         <v>61.2</v>
       </c>
-      <c r="P47" s="4"/>
+      <c r="P47" s="4">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>183</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>184</v>
+      </c>
+      <c r="P48" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sanity checks and a whole bunch of upgrades
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF474E9-D858-4010-A8B4-2752ECD19D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B4ED5F-4D67-4AFE-9FAF-E90D276B37BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
+    <workbookView xWindow="-28800" yWindow="345" windowWidth="28800" windowHeight="15240" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="193">
   <si>
     <t>Category</t>
   </si>
@@ -582,7 +582,31 @@
     <t>a029</t>
   </si>
   <si>
-    <t>(45)+tweak loader, fallbacks in simple, unlock t0</t>
+    <t>(44)+tweak loader, fallbacks in simple, unlock t0</t>
+  </si>
+  <si>
+    <t>(46)+regularization in simple and GP</t>
+  </si>
+  <si>
+    <t>(47)+force Kepler</t>
+  </si>
+  <si>
+    <t>(48)+fudge based on var</t>
+  </si>
+  <si>
+    <t>(49)+adjust based on u</t>
+  </si>
+  <si>
+    <t>Not using force Kepler</t>
+  </si>
+  <si>
+    <t>(47)+fudge based on var</t>
+  </si>
+  <si>
+    <t>(51)+adjust based on u</t>
+  </si>
+  <si>
+    <t>(52)+fudge based on multi, multi-transit</t>
   </si>
 </sst>
 </file>
@@ -690,8 +714,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:Q48" totalsRowShown="0">
-  <autoFilter ref="A1:Q48" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:Q55" totalsRowShown="0">
+  <autoFilter ref="A1:Q55" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -1403,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2940,7 +2964,131 @@
       <c r="D48" t="s">
         <v>184</v>
       </c>
-      <c r="P48" s="4"/>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48">
+        <v>0.61219999999999997</v>
+      </c>
+      <c r="P48" s="4">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49">
+        <v>0.62139999999999995</v>
+      </c>
+      <c r="P49" s="4">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>186</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50">
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="P50" s="4">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="D51" t="s">
+        <v>187</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51">
+        <v>0.63139999999999996</v>
+      </c>
+      <c r="P51" s="4"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52">
+        <v>0.63629999999999998</v>
+      </c>
+      <c r="P52" s="4"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="D53" t="s">
+        <v>190</v>
+      </c>
+      <c r="E53" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53">
+        <v>0.63029999999999997</v>
+      </c>
+      <c r="P53" s="4">
+        <v>0.61799999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="D54" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="P54" s="4">
+        <v>0.622</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="D55" t="s">
+        <v>192</v>
+      </c>
+      <c r="E55" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55">
+        <v>0.63990000000000002</v>
+      </c>
+      <c r="P55" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepare for new baseline
</commit_message>
<xml_diff>
--- a/choices.xlsx
+++ b/choices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ariel2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B4ED5F-4D67-4AFE-9FAF-E90D276B37BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F89C1A8-2E09-4584-B15C-173A683149D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="345" windowWidth="28800" windowHeight="15240" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
+    <workbookView xWindow="-28800" yWindow="345" windowWidth="28800" windowHeight="15135" activeTab="1" xr2:uid="{A07B647F-CF3A-4B09-9617-55BE27F02610}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="195">
   <si>
     <t>Category</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>(52)+fudge based on multi, multi-transit</t>
+  </si>
+  <si>
+    <t>(52)+outer multi</t>
+  </si>
+  <si>
+    <t>Partial</t>
   </si>
 </sst>
 </file>
@@ -714,8 +720,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:Q55" totalsRowShown="0">
-  <autoFilter ref="A1:Q55" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}" name="Table2" displayName="Table2" ref="A1:Q56" totalsRowShown="0">
+  <autoFilter ref="A1:Q56" xr:uid="{162C9714-ECF8-452D-98E8-68CBD3A0A6AF}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{CD0C5B4F-9DA5-4851-8175-AEDC1F5441EB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{96CE9708-90D1-445F-AD73-473D0FFF2A0B}" name="GIT"/>
@@ -1427,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421DFAC1-2EB9-4491-B20E-B2D987A1FB50}">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,7 +3094,21 @@
       <c r="G55">
         <v>0.63990000000000002</v>
       </c>
-      <c r="P55" s="4"/>
+      <c r="P55" s="4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="D56" t="s">
+        <v>193</v>
+      </c>
+      <c r="E56" t="s">
+        <v>194</v>
+      </c>
+      <c r="P56" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>